<commit_message>
Update from Brendan's laptop at end of meeting 1/14/20
</commit_message>
<xml_diff>
--- a/LandscapeExampleOutput.xlsx
+++ b/LandscapeExampleOutput.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scouting\Documents\2020Scouting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\team3641\2020\Scouting Laptop Github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DB06F7E-51EB-4A95-9662-9E8A958AB481}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5E7298-6AC7-4019-A481-173A512DB1E9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3312" yWindow="72" windowWidth="17280" windowHeight="10620" xr2:uid="{0866CB5C-787B-474D-A6AF-83F91867D0CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0866CB5C-787B-474D-A6AF-83F91867D0CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -247,12 +247,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -267,9 +273,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,33 +450,33 @@
     <tableColumn id="7" xr3:uid="{D304A1E9-960E-45EA-88B3-35A38FE642E6}" uniqueName="7" name="ATFS.Question023" queryTableFieldId="7" dataDxfId="27"/>
     <tableColumn id="8" xr3:uid="{C0AADF53-ECB2-49B6-901E-19B091CF9837}" uniqueName="8" name="ATNS.Question022" queryTableFieldId="8" dataDxfId="26"/>
     <tableColumn id="9" xr3:uid="{BDB9702B-F56D-4F79-AF78-FEFD64F1672E}" uniqueName="9" name="Accuracy.Question029" queryTableFieldId="9"/>
-    <tableColumn id="10" xr3:uid="{F5EF4AD6-1518-46FC-BB47-4AF0DCC449C3}" uniqueName="10" name="CIL.Question011" queryTableFieldId="10" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{BA812E80-0BD2-4AE9-9FE7-7202365CF3AB}" uniqueName="11" name="Climb Postion.Question028" queryTableFieldId="11" dataDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{BC5F116E-A3D8-4204-8BB6-E300A9954B9C}" uniqueName="12" name="Climb.Question027" queryTableFieldId="12" dataDxfId="23"/>
-    <tableColumn id="13" xr3:uid="{D43A3831-0DE2-4B9B-A888-D7F876A99879}" uniqueName="13" name="Defense.Question035" queryTableFieldId="13" dataDxfId="22"/>
-    <tableColumn id="14" xr3:uid="{06B0C8F1-0561-431F-A0C2-FEE8DC573725}" uniqueName="14" name="Match#.Question001" queryTableFieldId="14" dataDxfId="21"/>
-    <tableColumn id="15" xr3:uid="{5FF40D6C-3B75-4AC6-AD4D-F5A934D78810}" uniqueName="15" name="Match#.Question002" queryTableFieldId="15" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{F5EF4AD6-1518-46FC-BB47-4AF0DCC449C3}" uniqueName="10" name="CIL.Question011" queryTableFieldId="10" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{BA812E80-0BD2-4AE9-9FE7-7202365CF3AB}" uniqueName="11" name="Climb Postion.Question028" queryTableFieldId="11" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{BC5F116E-A3D8-4204-8BB6-E300A9954B9C}" uniqueName="12" name="Climb.Question027" queryTableFieldId="12" dataDxfId="25"/>
+    <tableColumn id="13" xr3:uid="{D43A3831-0DE2-4B9B-A888-D7F876A99879}" uniqueName="13" name="Defense.Question035" queryTableFieldId="13" dataDxfId="24"/>
+    <tableColumn id="14" xr3:uid="{06B0C8F1-0561-431F-A0C2-FEE8DC573725}" uniqueName="14" name="Match#.Question001" queryTableFieldId="14" dataDxfId="23"/>
+    <tableColumn id="15" xr3:uid="{5FF40D6C-3B75-4AC6-AD4D-F5A934D78810}" uniqueName="15" name="Match#.Question002" queryTableFieldId="15" dataDxfId="22"/>
     <tableColumn id="16" xr3:uid="{51333092-EADF-4C06-BD7C-66AB1734890B}" uniqueName="16" name="Match#.Question003" queryTableFieldId="16"/>
-    <tableColumn id="17" xr3:uid="{D15337C0-1314-418B-818E-100BBC7ACEEF}" uniqueName="17" name="Pick Up.Question036" queryTableFieldId="17" dataDxfId="19"/>
-    <tableColumn id="18" xr3:uid="{57AC5C6E-2F6B-4DD3-AA9A-7E44ADCA5CF7}" uniqueName="18" name="Played Defense.Question021" queryTableFieldId="18" dataDxfId="18"/>
-    <tableColumn id="19" xr3:uid="{5D1645D9-D91E-471C-ACD2-0A8A38C6332D}" uniqueName="19" name="Pocition Control.Question019" queryTableFieldId="19" dataDxfId="17"/>
-    <tableColumn id="20" xr3:uid="{B810A802-E90B-4EDE-B7FF-E8B1C427FF17}" uniqueName="20" name="Position R.Question010" queryTableFieldId="20" dataDxfId="16"/>
-    <tableColumn id="21" xr3:uid="{1A211E36-039B-4443-AF97-9425F413261A}" uniqueName="21" name="Postition B.Question009" queryTableFieldId="21" dataDxfId="15"/>
-    <tableColumn id="22" xr3:uid="{73D7CB80-DFF9-4F39-9A74-4291D50A6360}" uniqueName="22" name="Rotation Control.Question020" queryTableFieldId="22" dataDxfId="14"/>
-    <tableColumn id="23" xr3:uid="{301487F9-E9E8-4551-8DCB-E00F10CA1280}" uniqueName="23" name="Speed.Question034" queryTableFieldId="23" dataDxfId="13"/>
-    <tableColumn id="24" xr3:uid="{4C54B494-8465-4EEA-856B-BD1FDF548492}" uniqueName="24" name="THG.Question004" queryTableFieldId="24" dataDxfId="12"/>
-    <tableColumn id="25" xr3:uid="{C881E927-CFB7-432F-9A63-03CF9723D84B}" uniqueName="25" name="THG.Question005" queryTableFieldId="25" dataDxfId="11"/>
-    <tableColumn id="26" xr3:uid="{20CC6E0C-56AB-4085-B4DB-73E797D178A1}" uniqueName="26" name="THG.Question006" queryTableFieldId="26" dataDxfId="10"/>
-    <tableColumn id="27" xr3:uid="{B1C2979B-2E42-4608-874A-D7631B1A125B}" uniqueName="27" name="THG.Question007" queryTableFieldId="27" dataDxfId="9"/>
-    <tableColumn id="28" xr3:uid="{2384DBD3-D6E0-4CB1-BFAA-147CD87B6F98}" uniqueName="28" name="THG.Question008" queryTableFieldId="28" dataDxfId="8"/>
-    <tableColumn id="29" xr3:uid="{E1EB2168-E43E-4ECC-9CC5-92FDB1AC752C}" uniqueName="29" name="TLG.Question014" queryTableFieldId="29" dataDxfId="7"/>
-    <tableColumn id="30" xr3:uid="{43E47D8C-B830-4342-AA02-2BE80D49C291}" uniqueName="30" name="TLG.Question015" queryTableFieldId="30" dataDxfId="6"/>
-    <tableColumn id="31" xr3:uid="{C209B684-5BC6-4C73-87CA-4D1F01296C11}" uniqueName="31" name="TLG.Question016" queryTableFieldId="31" dataDxfId="5"/>
-    <tableColumn id="32" xr3:uid="{4EAB643F-6ADF-4709-BF37-A121EF2D1017}" uniqueName="32" name="TLG.Question017" queryTableFieldId="32" dataDxfId="4"/>
-    <tableColumn id="33" xr3:uid="{5F85D37C-3A9F-431C-B590-D29B497531EB}" uniqueName="33" name="TLG.Question018" queryTableFieldId="33" dataDxfId="3"/>
-    <tableColumn id="34" xr3:uid="{7A99E1A2-3B96-49D8-8583-999D4AEDBA4A}" uniqueName="34" name="Team#.Question030" queryTableFieldId="34" dataDxfId="2"/>
-    <tableColumn id="35" xr3:uid="{9BBB3DB2-B871-492D-AFB6-01901BD79DBB}" uniqueName="35" name="Team#.Question031" queryTableFieldId="35" dataDxfId="1"/>
-    <tableColumn id="36" xr3:uid="{8BBCFD32-92B8-4851-B2E8-D85F22779E43}" uniqueName="36" name="Team#.Question032" queryTableFieldId="36" dataDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{D15337C0-1314-418B-818E-100BBC7ACEEF}" uniqueName="17" name="Pick Up.Question036" queryTableFieldId="17" dataDxfId="21"/>
+    <tableColumn id="18" xr3:uid="{57AC5C6E-2F6B-4DD3-AA9A-7E44ADCA5CF7}" uniqueName="18" name="Played Defense.Question021" queryTableFieldId="18" dataDxfId="20"/>
+    <tableColumn id="19" xr3:uid="{5D1645D9-D91E-471C-ACD2-0A8A38C6332D}" uniqueName="19" name="Pocition Control.Question019" queryTableFieldId="19" dataDxfId="19"/>
+    <tableColumn id="20" xr3:uid="{B810A802-E90B-4EDE-B7FF-E8B1C427FF17}" uniqueName="20" name="Position R.Question010" queryTableFieldId="20" dataDxfId="18"/>
+    <tableColumn id="21" xr3:uid="{1A211E36-039B-4443-AF97-9425F413261A}" uniqueName="21" name="Postition B.Question009" queryTableFieldId="21" dataDxfId="17"/>
+    <tableColumn id="22" xr3:uid="{73D7CB80-DFF9-4F39-9A74-4291D50A6360}" uniqueName="22" name="Rotation Control.Question020" queryTableFieldId="22" dataDxfId="16"/>
+    <tableColumn id="23" xr3:uid="{301487F9-E9E8-4551-8DCB-E00F10CA1280}" uniqueName="23" name="Speed.Question034" queryTableFieldId="23" dataDxfId="15"/>
+    <tableColumn id="24" xr3:uid="{4C54B494-8465-4EEA-856B-BD1FDF548492}" uniqueName="24" name="THG.Question004" queryTableFieldId="24" dataDxfId="14"/>
+    <tableColumn id="25" xr3:uid="{C881E927-CFB7-432F-9A63-03CF9723D84B}" uniqueName="25" name="THG.Question005" queryTableFieldId="25" dataDxfId="13"/>
+    <tableColumn id="26" xr3:uid="{20CC6E0C-56AB-4085-B4DB-73E797D178A1}" uniqueName="26" name="THG.Question006" queryTableFieldId="26" dataDxfId="12"/>
+    <tableColumn id="27" xr3:uid="{B1C2979B-2E42-4608-874A-D7631B1A125B}" uniqueName="27" name="THG.Question007" queryTableFieldId="27" dataDxfId="11"/>
+    <tableColumn id="28" xr3:uid="{2384DBD3-D6E0-4CB1-BFAA-147CD87B6F98}" uniqueName="28" name="THG.Question008" queryTableFieldId="28" dataDxfId="10"/>
+    <tableColumn id="29" xr3:uid="{E1EB2168-E43E-4ECC-9CC5-92FDB1AC752C}" uniqueName="29" name="TLG.Question014" queryTableFieldId="29" dataDxfId="9"/>
+    <tableColumn id="30" xr3:uid="{43E47D8C-B830-4342-AA02-2BE80D49C291}" uniqueName="30" name="TLG.Question015" queryTableFieldId="30" dataDxfId="8"/>
+    <tableColumn id="31" xr3:uid="{C209B684-5BC6-4C73-87CA-4D1F01296C11}" uniqueName="31" name="TLG.Question016" queryTableFieldId="31" dataDxfId="7"/>
+    <tableColumn id="32" xr3:uid="{4EAB643F-6ADF-4709-BF37-A121EF2D1017}" uniqueName="32" name="TLG.Question017" queryTableFieldId="32" dataDxfId="6"/>
+    <tableColumn id="33" xr3:uid="{5F85D37C-3A9F-431C-B590-D29B497531EB}" uniqueName="33" name="TLG.Question018" queryTableFieldId="33" dataDxfId="5"/>
+    <tableColumn id="34" xr3:uid="{7A99E1A2-3B96-49D8-8583-999D4AEDBA4A}" uniqueName="34" name="Team#.Question030" queryTableFieldId="34" dataDxfId="4"/>
+    <tableColumn id="35" xr3:uid="{9BBB3DB2-B871-492D-AFB6-01901BD79DBB}" uniqueName="35" name="Team#.Question031" queryTableFieldId="35" dataDxfId="3"/>
+    <tableColumn id="36" xr3:uid="{8BBCFD32-92B8-4851-B2E8-D85F22779E43}" uniqueName="36" name="Team#.Question032" queryTableFieldId="36" dataDxfId="2"/>
     <tableColumn id="37" xr3:uid="{1D54B4C5-6F10-4C8D-A5C8-EB7B09FD5D6A}" uniqueName="37" name="Team#.Question033" queryTableFieldId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -775,38 +782,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEB6D34-05B7-4D9C-AF5B-DF25E5061C79}">
   <dimension ref="A1:AK11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="21" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="49.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="29" max="33" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="37" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="33" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="37" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -919,7 +928,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>200</v>
       </c>
@@ -932,7 +941,7 @@
       <c r="E2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -944,19 +953,19 @@
       <c r="I2">
         <v>100</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>40</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="2" t="s">
         <v>40</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="2" t="s">
         <v>42</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -968,7 +977,7 @@
       <c r="R2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="2" t="s">
         <v>44</v>
       </c>
       <c r="T2" s="1" t="s">
@@ -983,7 +992,7 @@
       <c r="W2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="X2" s="2" t="s">
         <v>46</v>
       </c>
       <c r="Y2" s="1" t="s">
@@ -1013,10 +1022,10 @@
       <c r="AG2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AH2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AI2" s="2" t="s">
         <v>42</v>
       </c>
       <c r="AJ2" s="1" t="s">
@@ -1026,7 +1035,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>201</v>
       </c>
@@ -1039,25 +1048,25 @@
       <c r="E3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="I3">
         <v>100</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>40</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="2" t="s">
         <v>40</v>
       </c>
       <c r="M3" s="1" t="s">
@@ -1078,7 +1087,7 @@
       <c r="R3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="2" t="s">
         <v>44</v>
       </c>
       <c r="T3" s="1" t="s">
@@ -1093,10 +1102,10 @@
       <c r="W3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="X3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Y3" s="2" t="s">
         <v>50</v>
       </c>
       <c r="Z3" s="1" t="s">
@@ -1123,7 +1132,7 @@
       <c r="AG3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AH3" s="1" t="s">
+      <c r="AH3" s="2" t="s">
         <v>42</v>
       </c>
       <c r="AI3" s="1" t="s">
@@ -1136,7 +1145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>202</v>
       </c>
@@ -1152,7 +1161,7 @@
       <c r="F4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1161,19 +1170,19 @@
       <c r="I4">
         <v>100</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="2" t="s">
         <v>40</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="2" t="s">
         <v>40</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="2" t="s">
         <v>42</v>
       </c>
       <c r="O4" s="1" t="s">
@@ -1188,7 +1197,7 @@
       <c r="R4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="S4" s="2" t="s">
         <v>44</v>
       </c>
       <c r="T4" s="1" t="s">
@@ -1203,7 +1212,7 @@
       <c r="W4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="X4" s="2" t="s">
         <v>50</v>
       </c>
       <c r="Y4" s="1" t="s">
@@ -1224,7 +1233,7 @@
       <c r="AD4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AE4" s="2" t="s">
         <v>51</v>
       </c>
       <c r="AF4" s="1" t="s">
@@ -1246,14 +1255,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>203</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -1271,7 +1280,7 @@
       <c r="I5">
         <v>75</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="2" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -1283,7 +1292,7 @@
       <c r="M5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="2" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="1" t="s">
@@ -1292,10 +1301,10 @@
       <c r="P5">
         <v>2</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="R5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="S5" s="1" t="s">
@@ -1319,7 +1328,7 @@
       <c r="Y5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="Z5" s="2" t="s">
         <v>51</v>
       </c>
       <c r="AA5" s="1" t="s">
@@ -1337,7 +1346,7 @@
       <c r="AE5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AF5" s="1" t="s">
+      <c r="AF5" s="2" t="s">
         <v>56</v>
       </c>
       <c r="AG5" s="1" t="s">
@@ -1356,7 +1365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>204</v>
       </c>
@@ -1390,7 +1399,7 @@
       <c r="L6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="2" t="s">
         <v>44</v>
       </c>
       <c r="N6" s="1" t="s">
@@ -1402,7 +1411,7 @@
       <c r="P6">
         <v>2</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="2" t="s">
         <v>44</v>
       </c>
       <c r="R6" s="1" t="s">
@@ -1417,7 +1426,7 @@
       <c r="U6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="V6" s="2" t="s">
         <v>44</v>
       </c>
       <c r="W6" s="1" t="s">
@@ -1426,10 +1435,10 @@
       <c r="X6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="Y6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="Z6" s="1" t="s">
+      <c r="Z6" s="2" t="s">
         <v>56</v>
       </c>
       <c r="AA6" s="1" t="s">
@@ -1444,7 +1453,7 @@
       <c r="AD6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AE6" s="1" t="s">
+      <c r="AE6" s="2" t="s">
         <v>51</v>
       </c>
       <c r="AF6" s="1" t="s">
@@ -1453,20 +1462,20 @@
       <c r="AG6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AH6" s="1" t="s">
+      <c r="AH6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AI6" s="1" t="s">
+      <c r="AI6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AJ6" s="1" t="s">
+      <c r="AJ6" s="2" t="s">
         <v>42</v>
       </c>
       <c r="AK6">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>205</v>
       </c>
@@ -1479,7 +1488,7 @@
       <c r="E7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>39</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1491,19 +1500,19 @@
       <c r="I7">
         <v>25</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="2" t="s">
         <v>40</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="2" t="s">
         <v>42</v>
       </c>
       <c r="O7" s="1" t="s">
@@ -1521,7 +1530,7 @@
       <c r="S7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="T7" s="2" t="s">
         <v>44</v>
       </c>
       <c r="U7" s="1" t="s">
@@ -1530,7 +1539,7 @@
       <c r="V7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="W7" s="2" t="s">
         <v>44</v>
       </c>
       <c r="X7" s="1" t="s">
@@ -1554,10 +1563,10 @@
       <c r="AD7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AE7" s="1" t="s">
+      <c r="AE7" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AF7" s="1" t="s">
+      <c r="AF7" s="2" t="s">
         <v>56</v>
       </c>
       <c r="AG7" s="1" t="s">
@@ -1576,7 +1585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>206</v>
       </c>
@@ -1622,7 +1631,7 @@
       <c r="P8">
         <v>3</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="2" t="s">
         <v>44</v>
       </c>
       <c r="R8" s="1" t="s">
@@ -1640,7 +1649,7 @@
       <c r="V8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="W8" s="2" t="s">
         <v>44</v>
       </c>
       <c r="X8" s="1" t="s">
@@ -1658,13 +1667,13 @@
       <c r="AB8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC8" s="1" t="s">
+      <c r="AC8" s="2" t="s">
         <v>58</v>
       </c>
       <c r="AD8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AE8" s="1" t="s">
+      <c r="AE8" s="2" t="s">
         <v>51</v>
       </c>
       <c r="AF8" s="1" t="s">
@@ -1673,10 +1682,10 @@
       <c r="AG8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AH8" s="1" t="s">
+      <c r="AH8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AI8" s="1" t="s">
+      <c r="AI8" s="2" t="s">
         <v>42</v>
       </c>
       <c r="AJ8" s="1" t="s">
@@ -1686,7 +1695,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>207</v>
       </c>
@@ -1699,7 +1708,7 @@
       <c r="D9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -1714,19 +1723,19 @@
       <c r="I9">
         <v>75</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="2" t="s">
         <v>40</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L9" s="2" t="s">
         <v>40</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N9" s="2" t="s">
         <v>42</v>
       </c>
       <c r="O9" s="1" t="s">
@@ -1747,22 +1756,22 @@
       <c r="T9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="U9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="V9" s="2" t="s">
         <v>44</v>
       </c>
       <c r="W9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="X9" s="1" t="s">
+      <c r="X9" s="2" t="s">
         <v>61</v>
       </c>
       <c r="Y9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Z9" s="1" t="s">
+      <c r="Z9" s="2" t="s">
         <v>51</v>
       </c>
       <c r="AA9" s="1" t="s">
@@ -1786,10 +1795,10 @@
       <c r="AG9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AH9" s="1" t="s">
+      <c r="AH9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AI9" s="1" t="s">
+      <c r="AI9" s="2" t="s">
         <v>42</v>
       </c>
       <c r="AJ9" s="1" t="s">
@@ -1799,7 +1808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>208</v>
       </c>
@@ -1818,7 +1827,7 @@
       <c r="F10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -1827,13 +1836,13 @@
       <c r="I10">
         <v>75</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="2" t="s">
         <v>40</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" s="2" t="s">
         <v>40</v>
       </c>
       <c r="M10" s="1" t="s">
@@ -1842,13 +1851,13 @@
       <c r="N10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="2" t="s">
         <v>62</v>
       </c>
       <c r="P10">
         <v>4</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" s="2" t="s">
         <v>44</v>
       </c>
       <c r="R10" s="1" t="s">
@@ -1863,19 +1872,19 @@
       <c r="U10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="V10" s="2" t="s">
         <v>44</v>
       </c>
       <c r="W10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="X10" s="1" t="s">
+      <c r="X10" s="2" t="s">
         <v>51</v>
       </c>
       <c r="Y10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="Z10" s="1" t="s">
+      <c r="Z10" s="2" t="s">
         <v>56</v>
       </c>
       <c r="AA10" s="1" t="s">
@@ -1884,7 +1893,7 @@
       <c r="AB10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC10" s="1" t="s">
+      <c r="AC10" s="2" t="s">
         <v>56</v>
       </c>
       <c r="AD10" s="1" t="s">
@@ -1896,13 +1905,13 @@
       <c r="AF10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AG10" s="1" t="s">
+      <c r="AG10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AH10" s="1" t="s">
+      <c r="AH10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AI10" s="1" t="s">
+      <c r="AI10" s="2" t="s">
         <v>42</v>
       </c>
       <c r="AJ10" s="1" t="s">
@@ -1912,7 +1921,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>209</v>
       </c>
@@ -1943,7 +1952,7 @@
       <c r="K11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L11" s="2" t="s">
         <v>40</v>
       </c>
       <c r="M11" s="1" t="s">
@@ -1985,7 +1994,7 @@
       <c r="Y11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Z11" s="1" t="s">
+      <c r="Z11" s="2" t="s">
         <v>58</v>
       </c>
       <c r="AA11" s="1" t="s">
@@ -1994,7 +2003,7 @@
       <c r="AB11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC11" s="1" t="s">
+      <c r="AC11" s="2" t="s">
         <v>46</v>
       </c>
       <c r="AD11" s="1" t="s">
@@ -2015,7 +2024,7 @@
       <c r="AI11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AJ11" s="1" t="s">
+      <c r="AJ11" s="2" t="s">
         <v>42</v>
       </c>
       <c r="AK11">
@@ -2024,8 +2033,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2036,7 +2046,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>